<commit_message>
Change in Run Mode
</commit_message>
<xml_diff>
--- a/src/com/Optimus_Poc/xls/Test_Cases_1.xlsx
+++ b/src/com/Optimus_Poc/xls/Test_Cases_1.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Gmail Automation (1)\ToBeUploaded on GH\SeleniumDemo\src\com\Optimus_Poc\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="888" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="888"/>
   </bookViews>
   <sheets>
-    <sheet name="Pre-requisites" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Test Cases" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Test Steps" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Pre-requisites" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Steps" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -187,35 +191,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,124 +221,348 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill>
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="33.0" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="42.4234693877551" collapsed="true"/>
-    <col min="3" max="1025" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
+    <col min="1" max="1" width="33" collapsed="1"/>
+    <col min="2" max="2" width="42.42578125" collapsed="1"/>
+    <col min="3" max="1025" width="8.7109375" collapsed="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -361,7 +571,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -370,7 +580,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -379,7 +589,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -388,16 +598,16 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -405,38 +615,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="D1" activeCellId="0" pane="topLeft" sqref="D1"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="46.5714285714286" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="61.9948979591837" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="0" width="27.09765625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="0" width="9.1640625" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
+    <col min="1" max="1" width="46.5703125" collapsed="1"/>
+    <col min="2" max="2" width="62" collapsed="1"/>
+    <col min="3" max="3" width="8.7109375" collapsed="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="1025" width="8.7109375" collapsed="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -446,14 +648,14 @@
       <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="8">
+      <c r="D1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s" s="10">
+      <c r="E1" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -470,7 +672,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -484,67 +686,59 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="6" width="41.4948979591837" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="6" width="8.6734693877551" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="6" width="52.0" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="6" width="31.1479591836735" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="6" width="44.9948979591837" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="6" width="22.0051020408163" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" hidden="false" style="6" width="7.51171875" collapsed="true"/>
-    <col min="8" max="1018" hidden="false" style="6" width="8.6734693877551" collapsed="true"/>
-    <col min="1019" max="1025" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
+    <col min="1" max="1" width="41.42578125" style="6" collapsed="1"/>
+    <col min="2" max="2" width="8.7109375" style="6" collapsed="1"/>
+    <col min="3" max="3" width="52" style="6" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" style="6" collapsed="1"/>
+    <col min="5" max="5" width="45" style="6" collapsed="1"/>
+    <col min="6" max="6" width="22" style="6" collapsed="1"/>
+    <col min="7" max="7" width="7.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="1018" width="8.7109375" style="6" collapsed="1"/>
+    <col min="1019" max="1025" width="8.7109375" collapsed="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -563,11 +757,11 @@
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="9">
+      <c r="G1" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -588,7 +782,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -609,7 +803,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="4">
+    <row r="4" spans="1:7" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -628,7 +822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="5">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -649,7 +843,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="6">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -672,7 +866,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="7">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -693,7 +887,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -712,7 +906,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -730,7 +924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -748,7 +942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -764,7 +958,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -782,7 +976,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -802,7 +996,7 @@
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -820,7 +1014,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -836,8 +1030,8 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -854,8 +1048,8 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -872,8 +1066,8 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -888,8 +1082,8 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -906,8 +1100,8 @@
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -926,8 +1120,8 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -944,8 +1138,8 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -960,8 +1154,8 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -978,8 +1172,8 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -996,8 +1190,8 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1012,8 +1206,8 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1030,8 +1224,8 @@
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1050,8 +1244,8 @@
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1068,8 +1262,8 @@
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1085,12 +1279,7 @@
       <c r="F33" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>